<commit_message>
major structure changes and delta corrections
</commit_message>
<xml_diff>
--- a/src/ar/edu/itba/sia/group3/TP3-ej2-Conjunto_entrenamiento.xlsx
+++ b/src/ar/edu/itba/sia/group3/TP3-ej2-Conjunto_entrenamiento.xlsx
@@ -235,7 +235,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="A2:D30"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -247,19 +247,32 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
+      <c r="A2" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>21.7550223576887</v>
       </c>
       <c r="F2" s="0"/>
     </row>
@@ -268,13 +281,13 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>-0.8</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>0</v>
-      </c>
       <c r="D3" s="7" t="n">
-        <v>21.7550223576887</v>
+        <v>7.17575422637513</v>
       </c>
       <c r="F3" s="0"/>
     </row>
@@ -283,58 +296,58 @@
         <v>1.2</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>-0.8</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>7.17575422637513</v>
+        <v>43.0453776060771</v>
       </c>
       <c r="F4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>1.2</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="C5" s="6" t="n">
         <v>-0.8</v>
       </c>
-      <c r="C5" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="D5" s="7" t="n">
-        <v>43.0453776060771</v>
+        <v>2.874849592654</v>
       </c>
       <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.874849592654</v>
+        <v>26.5027400533481</v>
       </c>
       <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <v>7.9</v>
+        <v>0.4</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>26.5027400533481</v>
+        <v>68.5680113938254</v>
       </c>
       <c r="F7" s="0"/>
       <c r="N7" s="0" t="s">
@@ -343,46 +356,46 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <v>0.4</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>0</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>2.7</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>68.5680113938254</v>
+        <v>61.3014176139336</v>
       </c>
       <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>0</v>
+        <v>-1.3</v>
       </c>
       <c r="B9" s="6" t="n">
-        <v>0.4</v>
+        <v>3.23</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>61.3014176139336</v>
+        <v>23.1831196442489</v>
       </c>
       <c r="F9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <v>-1.3</v>
+        <v>0.4</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>3.23</v>
+        <v>2.7</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>23.1831196442489</v>
+        <v>2.81952879701426</v>
       </c>
       <c r="F10" s="0"/>
     </row>
@@ -394,25 +407,25 @@
         <v>2.7</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>2.81952879701426</v>
+        <v>17.6535274779117</v>
       </c>
       <c r="F11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
-        <v>0.4</v>
+        <v>-1.3</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>2</v>
+        <v>3.23</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>17.6535274779117</v>
+        <v>72.5119497789823</v>
       </c>
       <c r="F12" s="0"/>
       <c r="N12" s="0" t="s">
@@ -421,61 +434,61 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="n">
         <v>-1.3</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>0</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>3.23</v>
       </c>
       <c r="D13" s="7" t="n">
-        <v>72.5119497789823</v>
+        <v>88.184302219073</v>
       </c>
       <c r="F13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>-1.3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>3.23</v>
+        <v>-2</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>88.184302219073</v>
+        <v>4.65304745147315</v>
       </c>
       <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
-        <v>7.9</v>
+        <v>1.8</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>-2</v>
+        <v>1.6</v>
       </c>
       <c r="D15" s="7" t="n">
-        <v>4.65304745147315</v>
+        <v>49.0001333120035</v>
       </c>
       <c r="F15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="B16" s="6" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="D16" s="7" t="n">
-        <v>49.0001333120035</v>
+        <v>76.8524783499018</v>
       </c>
       <c r="F16" s="0"/>
       <c r="N16" s="0" t="s">
@@ -484,121 +497,121 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>-2</v>
+        <v>0.6</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>76.8524783499018</v>
+        <v>7.87103371705352</v>
       </c>
       <c r="F17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="B18" s="6" t="n">
-        <v>0.6</v>
+        <v>1.8</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="D18" s="7" t="n">
-        <v>7.87103371705352</v>
+        <v>18.5427419292982</v>
       </c>
       <c r="F18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B19" s="6" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>18.5427419292982</v>
+        <v>2.65969935768659</v>
       </c>
       <c r="F19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <v>-2</v>
+        <v>-0.5</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D20" s="7" t="n">
-        <v>2.65969935768659</v>
+        <v>50.9998666879966</v>
       </c>
       <c r="F20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <v>-0.5</v>
+        <v>7.9</v>
       </c>
       <c r="B21" s="6" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D21" s="7" t="n">
-        <v>50.9998666879966</v>
+        <v>64.1067406334817</v>
       </c>
       <c r="F21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <v>7.9</v>
+        <v>-1.3</v>
       </c>
       <c r="B22" s="6" t="n">
-        <v>0</v>
+        <v>3.23</v>
       </c>
       <c r="C22" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="7" t="n">
-        <v>64.1067406334817</v>
+        <v>1.48031714816855</v>
       </c>
       <c r="F22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <v>-1.3</v>
+        <v>0</v>
       </c>
       <c r="B23" s="6" t="n">
-        <v>3.23</v>
+        <v>7.9</v>
       </c>
       <c r="C23" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="7" t="n">
-        <v>1.48031714816855</v>
+        <v>0.320446665755688</v>
       </c>
       <c r="F23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B24" s="6" t="n">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="C24" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="7" t="n">
-        <v>0.320446665755688</v>
+        <v>40.1312339887548</v>
       </c>
       <c r="F24" s="0"/>
     </row>
@@ -607,91 +620,77 @@
         <v>-2</v>
       </c>
       <c r="B25" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C25" s="6" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D25" s="7" t="n">
-        <v>40.1312339887548</v>
+        <v>0.995180186690432</v>
       </c>
       <c r="F25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="B26" s="6" t="n">
-        <v>2</v>
+        <v>-0.5</v>
       </c>
       <c r="C26" s="6" t="n">
-        <v>-1</v>
+        <v>0.6</v>
       </c>
       <c r="D26" s="7" t="n">
-        <v>0.995180186690432</v>
+        <v>24.9739894404882</v>
       </c>
       <c r="F26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="B27" s="6" t="n">
-        <v>-0.5</v>
+        <v>1.6</v>
       </c>
       <c r="C27" s="6" t="n">
-        <v>0.6</v>
+        <v>1.3</v>
       </c>
       <c r="D27" s="7" t="n">
-        <v>24.9739894404882</v>
+        <v>21.4165016957441</v>
       </c>
       <c r="F27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>18.2425523806356</v>
+      </c>
+      <c r="F28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="n">
         <v>1.8</v>
       </c>
-      <c r="B28" s="6" t="n">
+      <c r="B29" s="9" t="n">
         <v>1.6</v>
       </c>
-      <c r="C28" s="6" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="D28" s="7" t="n">
-        <v>21.4165016957441</v>
-      </c>
-      <c r="F28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="B29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>18.2425523806356</v>
+      <c r="C29" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10" t="n">
+        <v>6.91384203433468</v>
       </c>
       <c r="F29" s="0"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="B30" s="9" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="C30" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10" t="n">
-        <v>6.91384203433468</v>
-      </c>
-      <c r="F30" s="0"/>
-    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -711,7 +710,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:D30 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,7 +736,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:D30 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>